<commit_message>
Updated 9th Feb, 2017 version 1
</commit_message>
<xml_diff>
--- a/ReportingStructure/resource/Keywords.xlsx
+++ b/ReportingStructure/resource/Keywords.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
   <si>
     <t>KEY_WORDS</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>Verify text present inside table</t>
+  </si>
+  <si>
+    <t>CHANGE_CSS_ATTRIBUTE</t>
+  </si>
+  <si>
+    <t>Changing css attribute using javascript executor</t>
   </si>
 </sst>
 </file>
@@ -561,7 +567,7 @@
   <dimension ref="A1:E482"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,10 +835,10 @@
         <v>36</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="C16" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>38</v>
@@ -906,11 +912,21 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="5"/>
+      <c r="A21" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="5">
+        <v>100</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>

</xml_diff>